<commit_message>
added percentile ranges and notes to P4 & P5 frames sheets
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/frames for P4.xlsx
+++ b/Dataset Excel Sheets/Frames/frames for P4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\Desktop\Senior Design\CSE 491 - Senior Design II\github\Senior-Design-Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/Frames/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4252DDE4-3589-46C8-A570-F1EC832A9924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4252DDE4-3589-46C8-A570-F1EC832A9924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07231359-F015-4C6F-A927-120FFC52A7C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="372" yWindow="24" windowWidth="21732" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>count</t>
   </si>
@@ -52,12 +52,36 @@
   <si>
     <t>25%-75%</t>
   </si>
+  <si>
+    <t>2: [66, 90]</t>
+  </si>
+  <si>
+    <t>3: [100, 126]</t>
+  </si>
+  <si>
+    <t>4: [129, 169]</t>
+  </si>
+  <si>
+    <t>5: [147, 184]</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>No overlap between 2 &amp; 3</t>
+  </si>
+  <si>
+    <t>No overlap between 3 &amp; 4</t>
+  </si>
+  <si>
+    <t>Small overlap between 4 &amp; 5 (22 frames)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +103,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -274,7 +306,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L470"/>
+  <dimension ref="A1:N470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,9 +624,11 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -604,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>60</v>
       </c>
@@ -630,11 +668,14 @@
       <c r="J2" s="5">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N2" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>63</v>
       </c>
@@ -662,9 +703,14 @@
       <c r="J3" s="7">
         <v>198</v>
       </c>
-      <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>63</v>
       </c>
@@ -692,9 +738,14 @@
       <c r="J4" s="7">
         <v>167.055556</v>
       </c>
-      <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>58</v>
       </c>
@@ -722,9 +773,14 @@
       <c r="J5" s="7">
         <v>25.075965</v>
       </c>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>58</v>
       </c>
@@ -752,9 +808,11 @@
       <c r="J6" s="7">
         <v>118</v>
       </c>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>62</v>
       </c>
@@ -783,7 +841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>54</v>
       </c>
@@ -812,7 +870,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>56</v>
       </c>
@@ -841,7 +899,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>57</v>
       </c>
@@ -870,7 +928,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>64</v>
       </c>
@@ -884,7 +942,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>61</v>
       </c>
@@ -898,7 +956,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>57</v>
       </c>
@@ -912,7 +970,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>55</v>
       </c>
@@ -926,7 +984,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>69</v>
       </c>
@@ -940,7 +998,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>59</v>
       </c>

</xml_diff>